<commit_message>
Update Check List SDD v 3.0 (1).xlsx
</commit_message>
<xml_diff>
--- a/Documenti/SDD/Check List SDD v 3.0 (1).xlsx
+++ b/Documenti/SDD/Check List SDD v 3.0 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRAA\Documenti\SDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisalerno-my.sharepoint.com/personal/a_afeltra12_studenti_unisa_it/Documents/GitHub/FRAA/Documenti/SDD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9B8BE1-91C3-456B-8314-3DE9D91888C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4C9B8BE1-91C3-456B-8314-3DE9D91888C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01EB9265-9DD6-45FA-B773-DE5E4634414F}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="2835" windowWidth="15870" windowHeight="9825" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check-list SDD" sheetId="1" r:id="rId1"/>
@@ -1013,58 +1013,147 @@
     <xf numFmtId="9" fontId="4" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="15" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1102,6 +1191,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1121,6 +1222,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1139,127 +1243,23 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1631,21 +1631,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:LI122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="D85" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" customWidth="1"/>
+    <col min="4" max="4" width="68.73046875" customWidth="1"/>
+    <col min="5" max="5" width="6.1328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="10" t="s">
@@ -1654,17 +1654,17 @@
       <c r="E1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="82"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="113"/>
       <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="13">
@@ -1675,19 +1675,19 @@
         <f>COUNTIF(E15:E122, "NA")</f>
         <v>53</v>
       </c>
-      <c r="F2" s="83">
+      <c r="F2" s="114">
         <f>COUNTIF(F15:I122, "NO")</f>
         <v>53</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="116"/>
       <c r="J2" s="14" t="str">
         <f>IF((D2+E2+F2)=53, OK, "Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte")</f>
         <v>Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D3" s="15"/>
       <c r="E3" s="9"/>
       <c r="F3" s="8">
@@ -1706,7 +1706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="19">
@@ -1730,23 +1730,23 @@
         <v>Controlla se hai cancellato tutte le voci che non servono</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="105" t="s">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-    </row>
-    <row r="8" spans="2:10" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
+      <c r="I6" s="142"/>
+    </row>
+    <row r="8" spans="2:10" ht="20.65" x14ac:dyDescent="0.6">
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1757,48 +1757,48 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="2:10" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="2"/>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="100"/>
-      <c r="E10" s="94" t="s">
+      <c r="D10" s="135"/>
+      <c r="E10" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="96"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="131"/>
       <c r="J10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="2"/>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="128"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
+      <c r="F11" s="146"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="146"/>
+      <c r="I11" s="146"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="133"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B13" s="2"/>
       <c r="C13" s="6" t="s">
         <v>3</v>
@@ -1806,52 +1806,52 @@
       <c r="D13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="86" t="s">
+      <c r="E13" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="88"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="119"/>
       <c r="J13" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:10" s="23" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" s="23" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="22"/>
       <c r="C14" s="24"/>
-      <c r="D14" s="73" t="s">
+      <c r="D14" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="74"/>
-    </row>
-    <row r="15" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="147"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
+      <c r="H14" s="147"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="148"/>
+    </row>
+    <row r="15" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
-      <c r="C15" s="64">
+      <c r="C15" s="70">
         <v>1</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="136" t="s">
         <v>50</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="64"/>
-    </row>
-    <row r="16" spans="2:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="65"/>
-      <c r="D16" s="101"/>
+      <c r="F15" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="122"/>
+      <c r="J15" s="70"/>
+    </row>
+    <row r="16" spans="2:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="71"/>
+      <c r="D16" s="137"/>
       <c r="E16" s="35" t="s">
         <v>8</v>
       </c>
@@ -1867,31 +1867,31 @@
       <c r="I16" s="58">
         <v>0.7</v>
       </c>
-      <c r="J16" s="65"/>
-    </row>
-    <row r="17" spans="2:10" s="46" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="71"/>
+    </row>
+    <row r="17" spans="2:10" s="46" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="45"/>
-      <c r="C17" s="64">
+      <c r="C17" s="70">
         <v>2</v>
       </c>
-      <c r="D17" s="66" t="s">
+      <c r="D17" s="136" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="64"/>
-    </row>
-    <row r="18" spans="2:10" s="46" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="125"/>
+      <c r="H17" s="125"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" spans="2:10" s="46" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="45"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="67"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="124"/>
       <c r="E18" s="44" t="s">
         <v>8</v>
       </c>
@@ -1907,31 +1907,31 @@
       <c r="I18" s="58">
         <v>0.7</v>
       </c>
-      <c r="J18" s="65"/>
-    </row>
-    <row r="19" spans="2:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="71"/>
+    </row>
+    <row r="19" spans="2:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
-      <c r="C19" s="64">
+      <c r="C19" s="70">
         <v>3</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="123" t="s">
         <v>60</v>
       </c>
       <c r="E19" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="69"/>
+      <c r="F19" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="125"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="126"/>
       <c r="J19" s="41"/>
     </row>
-    <row r="20" spans="2:10" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="55.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="67"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="124"/>
       <c r="E20" s="44" t="s">
         <v>8</v>
       </c>
@@ -1949,29 +1949,29 @@
       </c>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
-      <c r="C21" s="64">
+      <c r="C21" s="70">
         <v>4</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="123" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="64"/>
-    </row>
-    <row r="22" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="105"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="106"/>
+      <c r="J21" s="70"/>
+    </row>
+    <row r="22" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="67"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="124"/>
       <c r="E22" s="44" t="s">
         <v>8</v>
       </c>
@@ -1987,31 +1987,31 @@
       <c r="I22" s="58">
         <v>0.7</v>
       </c>
-      <c r="J22" s="65"/>
-    </row>
-    <row r="23" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="71"/>
+    </row>
+    <row r="23" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
-      <c r="C23" s="64">
+      <c r="C23" s="70">
         <v>5</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="123" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="64"/>
-    </row>
-    <row r="24" spans="2:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="70"/>
+    </row>
+    <row r="24" spans="2:10" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="67"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="124"/>
       <c r="E24" s="44" t="s">
         <v>8</v>
       </c>
@@ -2027,31 +2027,31 @@
       <c r="I24" s="59">
         <v>0.7</v>
       </c>
-      <c r="J24" s="65"/>
-    </row>
-    <row r="25" spans="2:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="71"/>
+    </row>
+    <row r="25" spans="2:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
-      <c r="C25" s="64">
-        <v>6</v>
-      </c>
-      <c r="D25" s="72" t="s">
+      <c r="C25" s="70">
+        <v>6</v>
+      </c>
+      <c r="D25" s="123" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="64"/>
-    </row>
-    <row r="26" spans="2:10" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="70"/>
+    </row>
+    <row r="26" spans="2:10" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="2"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="67"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="124"/>
       <c r="E26" s="28" t="s">
         <v>8</v>
       </c>
@@ -2067,31 +2067,31 @@
       <c r="I26" s="58">
         <v>0.7</v>
       </c>
-      <c r="J26" s="65"/>
-    </row>
-    <row r="27" spans="2:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="71"/>
+    </row>
+    <row r="27" spans="2:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
-      <c r="C27" s="64">
-        <v>7</v>
-      </c>
-      <c r="D27" s="72" t="s">
+      <c r="C27" s="70">
+        <v>7</v>
+      </c>
+      <c r="D27" s="123" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="64"/>
-    </row>
-    <row r="28" spans="2:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="70"/>
+    </row>
+    <row r="28" spans="2:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="22"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="67"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="124"/>
       <c r="E28" s="28" t="s">
         <v>8</v>
       </c>
@@ -2107,31 +2107,31 @@
       <c r="I28" s="58">
         <v>0.7</v>
       </c>
-      <c r="J28" s="65"/>
-    </row>
-    <row r="29" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="71"/>
+    </row>
+    <row r="29" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
-      <c r="C29" s="64">
-        <v>8</v>
-      </c>
-      <c r="D29" s="72" t="s">
+      <c r="C29" s="70">
+        <v>8</v>
+      </c>
+      <c r="D29" s="123" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="64"/>
-    </row>
-    <row r="30" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="125"/>
+      <c r="H29" s="125"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="70"/>
+    </row>
+    <row r="30" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="67"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="124"/>
       <c r="E30" s="44" t="s">
         <v>8</v>
       </c>
@@ -2147,31 +2147,31 @@
       <c r="I30" s="58">
         <v>0.7</v>
       </c>
-      <c r="J30" s="71"/>
-    </row>
-    <row r="31" spans="2:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="107"/>
+    </row>
+    <row r="31" spans="2:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
-      <c r="C31" s="64">
+      <c r="C31" s="70">
         <v>9</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D31" s="123" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="64"/>
-    </row>
-    <row r="32" spans="2:10" ht="58.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="105"/>
+      <c r="H31" s="105"/>
+      <c r="I31" s="106"/>
+      <c r="J31" s="70"/>
+    </row>
+    <row r="32" spans="2:10" ht="58.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="2"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="67"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="124"/>
       <c r="E32" s="44" t="s">
         <v>8</v>
       </c>
@@ -2187,31 +2187,31 @@
       <c r="I32" s="58">
         <v>0.7</v>
       </c>
-      <c r="J32" s="65"/>
-    </row>
-    <row r="33" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="71"/>
+    </row>
+    <row r="33" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
-      <c r="C33" s="64">
+      <c r="C33" s="70">
         <v>10</v>
       </c>
-      <c r="D33" s="66" t="s">
+      <c r="D33" s="136" t="s">
         <v>54</v>
       </c>
       <c r="E33" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="64"/>
-    </row>
-    <row r="34" spans="2:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="105"/>
+      <c r="H33" s="105"/>
+      <c r="I33" s="106"/>
+      <c r="J33" s="70"/>
+    </row>
+    <row r="34" spans="2:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="2"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="67"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="124"/>
       <c r="E34" s="28" t="s">
         <v>8</v>
       </c>
@@ -2224,42 +2224,42 @@
       <c r="H34" s="30">
         <v>0.5</v>
       </c>
-      <c r="I34" s="30">
-        <v>0.7</v>
-      </c>
-      <c r="J34" s="65"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I34" s="58">
+        <v>0.7</v>
+      </c>
+      <c r="J34" s="71"/>
+    </row>
+    <row r="35" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35" s="25"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="103"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="104"/>
-    </row>
-    <row r="36" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="64">
+      <c r="D35" s="138"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="139"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="139"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="140"/>
+    </row>
+    <row r="36" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="70">
         <v>11</v>
       </c>
-      <c r="D36" s="124" t="s">
+      <c r="D36" s="103" t="s">
         <v>45</v>
       </c>
       <c r="E36" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="64"/>
-    </row>
-    <row r="37" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="71"/>
-      <c r="D37" s="125"/>
+      <c r="F36" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="105"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="70"/>
+    </row>
+    <row r="37" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="107"/>
+      <c r="D37" s="104"/>
       <c r="E37" s="52" t="s">
         <v>8</v>
       </c>
@@ -2275,29 +2275,29 @@
       <c r="I37" s="58">
         <v>0.7</v>
       </c>
-      <c r="J37" s="65"/>
-    </row>
-    <row r="38" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="64">
+      <c r="J37" s="71"/>
+    </row>
+    <row r="38" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="70">
         <v>12</v>
       </c>
-      <c r="D38" s="124" t="s">
+      <c r="D38" s="103" t="s">
         <v>46</v>
       </c>
       <c r="E38" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="64"/>
-    </row>
-    <row r="39" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="71"/>
-      <c r="D39" s="125"/>
+      <c r="F38" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="105"/>
+      <c r="H38" s="105"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="70"/>
+    </row>
+    <row r="39" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="107"/>
+      <c r="D39" s="104"/>
       <c r="E39" s="52" t="s">
         <v>8</v>
       </c>
@@ -2313,29 +2313,29 @@
       <c r="I39" s="58">
         <v>0.7</v>
       </c>
-      <c r="J39" s="65"/>
-    </row>
-    <row r="40" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="64">
+      <c r="J39" s="71"/>
+    </row>
+    <row r="40" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="70">
         <v>13</v>
       </c>
-      <c r="D40" s="124" t="s">
+      <c r="D40" s="103" t="s">
         <v>47</v>
       </c>
       <c r="E40" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="64"/>
-    </row>
-    <row r="41" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="71"/>
-      <c r="D41" s="125"/>
+      <c r="F40" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="105"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="106"/>
+      <c r="J40" s="70"/>
+    </row>
+    <row r="41" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="107"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="52" t="s">
         <v>8</v>
       </c>
@@ -2345,35 +2345,35 @@
       <c r="G41" s="30">
         <v>0.3</v>
       </c>
-      <c r="H41" s="148">
-        <v>0.5</v>
-      </c>
-      <c r="I41" s="147">
-        <v>0.7</v>
-      </c>
-      <c r="J41" s="65"/>
-    </row>
-    <row r="42" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="64">
+      <c r="H41" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="61">
+        <v>0.7</v>
+      </c>
+      <c r="J41" s="71"/>
+    </row>
+    <row r="42" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="70">
         <v>14</v>
       </c>
-      <c r="D42" s="124" t="s">
+      <c r="D42" s="103" t="s">
         <v>48</v>
       </c>
       <c r="E42" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="64"/>
-    </row>
-    <row r="43" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="71"/>
-      <c r="D43" s="125"/>
+      <c r="F42" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="105"/>
+      <c r="H42" s="105"/>
+      <c r="I42" s="106"/>
+      <c r="J42" s="70"/>
+    </row>
+    <row r="43" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="107"/>
+      <c r="D43" s="104"/>
       <c r="E43" s="52" t="s">
         <v>8</v>
       </c>
@@ -2389,29 +2389,29 @@
       <c r="I43" s="58">
         <v>0.7</v>
       </c>
-      <c r="J43" s="65"/>
-    </row>
-    <row r="44" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="64">
+      <c r="J43" s="71"/>
+    </row>
+    <row r="44" spans="2:10" s="54" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="70">
         <v>15</v>
       </c>
-      <c r="D44" s="124" t="s">
+      <c r="D44" s="103" t="s">
         <v>49</v>
       </c>
       <c r="E44" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="64"/>
-    </row>
-    <row r="45" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="71"/>
-      <c r="D45" s="125"/>
+      <c r="F44" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="105"/>
+      <c r="H44" s="105"/>
+      <c r="I44" s="106"/>
+      <c r="J44" s="70"/>
+    </row>
+    <row r="45" spans="2:10" s="54" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C45" s="107"/>
+      <c r="D45" s="104"/>
       <c r="E45" s="52" t="s">
         <v>8</v>
       </c>
@@ -2424,12 +2424,12 @@
       <c r="H45" s="30">
         <v>0.5</v>
       </c>
-      <c r="I45" s="30">
-        <v>0.7</v>
-      </c>
-      <c r="J45" s="65"/>
-    </row>
-    <row r="46" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I45" s="58">
+        <v>0.7</v>
+      </c>
+      <c r="J45" s="71"/>
+    </row>
+    <row r="46" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46" s="47"/>
       <c r="D46" s="55" t="s">
         <v>63</v>
@@ -2441,28 +2441,28 @@
       <c r="I46" s="39"/>
       <c r="J46" s="40"/>
     </row>
-    <row r="47" spans="2:10" s="27" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" s="27" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="26"/>
-      <c r="C47" s="64">
+      <c r="C47" s="70">
         <v>16</v>
       </c>
-      <c r="D47" s="75" t="s">
+      <c r="D47" s="143" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="91"/>
-      <c r="J47" s="107"/>
-    </row>
-    <row r="48" spans="2:10" s="27" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="65"/>
-      <c r="D48" s="76"/>
+      <c r="F47" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="121"/>
+      <c r="H47" s="121"/>
+      <c r="I47" s="122"/>
+      <c r="J47" s="63"/>
+    </row>
+    <row r="48" spans="2:10" s="27" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C48" s="71"/>
+      <c r="D48" s="144"/>
       <c r="E48" s="34" t="s">
         <v>8</v>
       </c>
@@ -2478,31 +2478,31 @@
       <c r="I48" s="58">
         <v>0.7</v>
       </c>
-      <c r="J48" s="108"/>
-    </row>
-    <row r="49" spans="2:10" s="27" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J48" s="64"/>
+    </row>
+    <row r="49" spans="2:10" s="27" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="26"/>
-      <c r="C49" s="64">
+      <c r="C49" s="70">
         <v>17</v>
       </c>
-      <c r="D49" s="75" t="s">
+      <c r="D49" s="143" t="s">
         <v>24</v>
       </c>
       <c r="E49" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="109"/>
-      <c r="H49" s="109"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="107"/>
-    </row>
-    <row r="50" spans="2:10" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F49" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="63"/>
+    </row>
+    <row r="50" spans="2:10" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="26"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="77"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="145"/>
       <c r="E50" s="34" t="s">
         <v>8</v>
       </c>
@@ -2518,30 +2518,30 @@
       <c r="I50" s="58">
         <v>0.7</v>
       </c>
-      <c r="J50" s="108"/>
-    </row>
-    <row r="51" spans="2:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J50" s="64"/>
+    </row>
+    <row r="51" spans="2:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="36"/>
-      <c r="C51" s="64">
+      <c r="C51" s="70">
         <v>18</v>
       </c>
-      <c r="D51" s="78" t="s">
+      <c r="D51" s="108" t="s">
         <v>44</v>
       </c>
       <c r="E51" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="119" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="120"/>
-      <c r="H51" s="120"/>
-      <c r="I51" s="121"/>
-      <c r="J51" s="117"/>
-    </row>
-    <row r="52" spans="2:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="65"/>
-      <c r="D52" s="79"/>
+      <c r="F51" s="100" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="101"/>
+      <c r="H51" s="101"/>
+      <c r="I51" s="102"/>
+      <c r="J51" s="88"/>
+    </row>
+    <row r="52" spans="2:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C52" s="71"/>
+      <c r="D52" s="110"/>
       <c r="E52" s="34" t="s">
         <v>8</v>
       </c>
@@ -2557,30 +2557,30 @@
       <c r="I52" s="60">
         <v>0.7</v>
       </c>
-      <c r="J52" s="118"/>
-    </row>
-    <row r="53" spans="2:10" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="89"/>
+    </row>
+    <row r="53" spans="2:10" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="32"/>
-      <c r="C53" s="64">
+      <c r="C53" s="70">
         <v>19</v>
       </c>
-      <c r="D53" s="78" t="s">
+      <c r="D53" s="108" t="s">
         <v>43</v>
       </c>
       <c r="E53" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="119" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="120"/>
-      <c r="H53" s="120"/>
-      <c r="I53" s="121"/>
-      <c r="J53" s="117"/>
-    </row>
-    <row r="54" spans="2:10" s="31" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="65"/>
-      <c r="D54" s="114"/>
+      <c r="F53" s="100" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="101"/>
+      <c r="H53" s="101"/>
+      <c r="I53" s="102"/>
+      <c r="J53" s="88"/>
+    </row>
+    <row r="54" spans="2:10" s="31" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C54" s="71"/>
+      <c r="D54" s="109"/>
       <c r="E54" s="34" t="s">
         <v>8</v>
       </c>
@@ -2596,31 +2596,31 @@
       <c r="I54" s="60">
         <v>0.7</v>
       </c>
-      <c r="J54" s="118"/>
-    </row>
-    <row r="55" spans="2:10" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J54" s="89"/>
+    </row>
+    <row r="55" spans="2:10" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="56"/>
-      <c r="C55" s="64">
+      <c r="C55" s="70">
         <v>20</v>
       </c>
-      <c r="D55" s="115" t="s">
+      <c r="D55" s="96" t="s">
         <v>56</v>
       </c>
       <c r="E55" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="113"/>
-      <c r="J55" s="117"/>
-    </row>
-    <row r="56" spans="2:10" s="57" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F55" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="90"/>
+      <c r="H55" s="90"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="88"/>
+    </row>
+    <row r="56" spans="2:10" s="57" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="56"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="116"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="97"/>
       <c r="E56" s="34" t="s">
         <v>8</v>
       </c>
@@ -2636,31 +2636,31 @@
       <c r="I56" s="60">
         <v>0.7</v>
       </c>
-      <c r="J56" s="118"/>
-    </row>
-    <row r="57" spans="2:10" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J56" s="89"/>
+    </row>
+    <row r="57" spans="2:10" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="56"/>
-      <c r="C57" s="64">
+      <c r="C57" s="70">
         <v>21</v>
       </c>
-      <c r="D57" s="115" t="s">
+      <c r="D57" s="96" t="s">
         <v>55</v>
       </c>
       <c r="E57" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G57" s="112"/>
-      <c r="H57" s="112"/>
-      <c r="I57" s="113"/>
-      <c r="J57" s="117"/>
-    </row>
-    <row r="58" spans="2:10" s="57" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F57" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="90"/>
+      <c r="H57" s="90"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="88"/>
+    </row>
+    <row r="58" spans="2:10" s="57" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B58" s="56"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="116"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="97"/>
       <c r="E58" s="34" t="s">
         <v>8</v>
       </c>
@@ -2676,31 +2676,31 @@
       <c r="I58" s="60">
         <v>0.7</v>
       </c>
-      <c r="J58" s="118"/>
-    </row>
-    <row r="59" spans="2:10" s="31" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J58" s="89"/>
+    </row>
+    <row r="59" spans="2:10" s="31" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="32"/>
-      <c r="C59" s="64">
+      <c r="C59" s="70">
         <v>22</v>
       </c>
-      <c r="D59" s="115" t="s">
+      <c r="D59" s="96" t="s">
         <v>64</v>
       </c>
       <c r="E59" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G59" s="112"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="113"/>
-      <c r="J59" s="117"/>
-    </row>
-    <row r="60" spans="2:10" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F59" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="90"/>
+      <c r="H59" s="90"/>
+      <c r="I59" s="91"/>
+      <c r="J59" s="88"/>
+    </row>
+    <row r="60" spans="2:10" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="32"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="116"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="97"/>
       <c r="E60" s="34" t="s">
         <v>8</v>
       </c>
@@ -2716,31 +2716,31 @@
       <c r="I60" s="60">
         <v>0.7</v>
       </c>
-      <c r="J60" s="118"/>
-    </row>
-    <row r="61" spans="2:10" s="27" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J60" s="89"/>
+    </row>
+    <row r="61" spans="2:10" s="27" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="26"/>
-      <c r="C61" s="64">
+      <c r="C61" s="70">
         <v>23</v>
       </c>
-      <c r="D61" s="122" t="s">
+      <c r="D61" s="74" t="s">
         <v>25</v>
       </c>
       <c r="E61" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61" s="109"/>
-      <c r="H61" s="109"/>
-      <c r="I61" s="110"/>
-      <c r="J61" s="107"/>
-    </row>
-    <row r="62" spans="2:10" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F61" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="67"/>
+      <c r="J61" s="63"/>
+    </row>
+    <row r="62" spans="2:10" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B62" s="26"/>
-      <c r="C62" s="65"/>
-      <c r="D62" s="123"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="75"/>
       <c r="E62" s="34" t="s">
         <v>8</v>
       </c>
@@ -2756,31 +2756,31 @@
       <c r="I62" s="58">
         <v>0.7</v>
       </c>
-      <c r="J62" s="108"/>
-    </row>
-    <row r="63" spans="2:10" s="27" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J62" s="64"/>
+    </row>
+    <row r="63" spans="2:10" s="27" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B63" s="26"/>
-      <c r="C63" s="64">
+      <c r="C63" s="70">
         <v>24</v>
       </c>
-      <c r="D63" s="122" t="s">
+      <c r="D63" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E63" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F63" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G63" s="109"/>
-      <c r="H63" s="109"/>
-      <c r="I63" s="110"/>
-      <c r="J63" s="107"/>
-    </row>
-    <row r="64" spans="2:10" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F63" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="67"/>
+      <c r="J63" s="63"/>
+    </row>
+    <row r="64" spans="2:10" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B64" s="26"/>
-      <c r="C64" s="65"/>
-      <c r="D64" s="123"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="75"/>
       <c r="E64" s="34" t="s">
         <v>8</v>
       </c>
@@ -2796,31 +2796,31 @@
       <c r="I64" s="58">
         <v>0.7</v>
       </c>
-      <c r="J64" s="108"/>
-    </row>
-    <row r="65" spans="1:321" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J64" s="64"/>
+    </row>
+    <row r="65" spans="1:321" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="26"/>
-      <c r="C65" s="64">
+      <c r="C65" s="70">
         <v>25</v>
       </c>
-      <c r="D65" s="122" t="s">
+      <c r="D65" s="74" t="s">
         <v>57</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G65" s="109"/>
-      <c r="H65" s="109"/>
-      <c r="I65" s="110"/>
-      <c r="J65" s="107"/>
-    </row>
-    <row r="66" spans="1:321" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F65" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="66"/>
+      <c r="H65" s="66"/>
+      <c r="I65" s="67"/>
+      <c r="J65" s="63"/>
+    </row>
+    <row r="66" spans="1:321" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B66" s="26"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="123"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="75"/>
       <c r="E66" s="34" t="s">
         <v>8</v>
       </c>
@@ -2836,31 +2836,31 @@
       <c r="I66" s="58">
         <v>0.7</v>
       </c>
-      <c r="J66" s="108"/>
-    </row>
-    <row r="67" spans="1:321" s="27" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J66" s="64"/>
+    </row>
+    <row r="67" spans="1:321" s="27" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="26"/>
-      <c r="C67" s="64">
+      <c r="C67" s="70">
         <v>28</v>
       </c>
-      <c r="D67" s="122" t="s">
+      <c r="D67" s="74" t="s">
         <v>67</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F67" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G67" s="109"/>
-      <c r="H67" s="109"/>
-      <c r="I67" s="110"/>
-      <c r="J67" s="107"/>
-    </row>
-    <row r="68" spans="1:321" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F67" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" s="66"/>
+      <c r="H67" s="66"/>
+      <c r="I67" s="67"/>
+      <c r="J67" s="63"/>
+    </row>
+    <row r="68" spans="1:321" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B68" s="26"/>
-      <c r="C68" s="65"/>
-      <c r="D68" s="123"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="75"/>
       <c r="E68" s="34" t="s">
         <v>8</v>
       </c>
@@ -2876,31 +2876,31 @@
       <c r="I68" s="58">
         <v>0.7</v>
       </c>
-      <c r="J68" s="108"/>
-    </row>
-    <row r="69" spans="1:321" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J68" s="64"/>
+    </row>
+    <row r="69" spans="1:321" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="26"/>
-      <c r="C69" s="64">
+      <c r="C69" s="70">
         <v>29</v>
       </c>
-      <c r="D69" s="142" t="s">
+      <c r="D69" s="79" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F69" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G69" s="109"/>
-      <c r="H69" s="109"/>
-      <c r="I69" s="110"/>
-      <c r="J69" s="107"/>
-    </row>
-    <row r="70" spans="1:321" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F69" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="66"/>
+      <c r="H69" s="66"/>
+      <c r="I69" s="67"/>
+      <c r="J69" s="63"/>
+    </row>
+    <row r="70" spans="1:321" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="26"/>
-      <c r="C70" s="65"/>
-      <c r="D70" s="123"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="75"/>
       <c r="E70" s="34" t="s">
         <v>8</v>
       </c>
@@ -2916,31 +2916,31 @@
       <c r="I70" s="58">
         <v>0.7</v>
       </c>
-      <c r="J70" s="108"/>
-    </row>
-    <row r="71" spans="1:321" s="57" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J70" s="64"/>
+    </row>
+    <row r="71" spans="1:321" s="57" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="56"/>
-      <c r="C71" s="64">
+      <c r="C71" s="70">
         <v>30</v>
       </c>
-      <c r="D71" s="130" t="s">
+      <c r="D71" s="77" t="s">
         <v>58</v>
       </c>
       <c r="E71" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F71" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G71" s="112"/>
-      <c r="H71" s="112"/>
-      <c r="I71" s="113"/>
-      <c r="J71" s="117"/>
-    </row>
-    <row r="72" spans="1:321" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F71" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="90"/>
+      <c r="H71" s="90"/>
+      <c r="I71" s="91"/>
+      <c r="J71" s="88"/>
+    </row>
+    <row r="72" spans="1:321" s="57" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B72" s="56"/>
-      <c r="C72" s="65"/>
-      <c r="D72" s="131"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="98"/>
       <c r="E72" s="34" t="s">
         <v>8</v>
       </c>
@@ -2956,30 +2956,30 @@
       <c r="I72" s="60">
         <v>0.7</v>
       </c>
-      <c r="J72" s="118"/>
-    </row>
-    <row r="73" spans="1:321" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J72" s="89"/>
+    </row>
+    <row r="73" spans="1:321" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="56"/>
-      <c r="C73" s="64">
+      <c r="C73" s="70">
         <v>31</v>
       </c>
-      <c r="D73" s="130" t="s">
+      <c r="D73" s="77" t="s">
         <v>66</v>
       </c>
       <c r="E73" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F73" s="119" t="s">
-        <v>7</v>
-      </c>
-      <c r="G73" s="120"/>
-      <c r="H73" s="120"/>
-      <c r="I73" s="121"/>
-      <c r="J73" s="117"/>
-    </row>
-    <row r="74" spans="1:321" s="57" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C74" s="65"/>
-      <c r="D74" s="144"/>
+      <c r="F73" s="100" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="101"/>
+      <c r="H73" s="101"/>
+      <c r="I73" s="102"/>
+      <c r="J73" s="88"/>
+    </row>
+    <row r="74" spans="1:321" s="57" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C74" s="71"/>
+      <c r="D74" s="99"/>
       <c r="E74" s="34" t="s">
         <v>8</v>
       </c>
@@ -2992,34 +2992,34 @@
       <c r="H74" s="33">
         <v>0.5</v>
       </c>
-      <c r="I74" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="J74" s="118"/>
-    </row>
-    <row r="75" spans="1:321" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I74" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="J74" s="89"/>
+    </row>
+    <row r="75" spans="1:321" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="36"/>
-      <c r="C75" s="64">
+      <c r="C75" s="70">
         <v>32</v>
       </c>
-      <c r="D75" s="130" t="s">
+      <c r="D75" s="77" t="s">
         <v>33</v>
       </c>
       <c r="E75" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G75" s="128"/>
-      <c r="H75" s="128"/>
-      <c r="I75" s="129"/>
-      <c r="J75" s="117"/>
-    </row>
-    <row r="76" spans="1:321" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F75" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="81"/>
+      <c r="H75" s="81"/>
+      <c r="I75" s="82"/>
+      <c r="J75" s="88"/>
+    </row>
+    <row r="76" spans="1:321" s="37" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B76" s="36"/>
-      <c r="C76" s="65"/>
-      <c r="D76" s="146"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="78"/>
       <c r="E76" s="34" t="s">
         <v>8</v>
       </c>
@@ -3035,31 +3035,31 @@
       <c r="I76" s="60">
         <v>0.7</v>
       </c>
-      <c r="J76" s="118"/>
-    </row>
-    <row r="77" spans="1:321" s="37" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J76" s="89"/>
+    </row>
+    <row r="77" spans="1:321" s="37" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="36"/>
-      <c r="C77" s="64">
+      <c r="C77" s="70">
         <v>33</v>
       </c>
-      <c r="D77" s="126" t="s">
+      <c r="D77" s="94" t="s">
         <v>59</v>
       </c>
       <c r="E77" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77" s="128"/>
-      <c r="H77" s="128"/>
-      <c r="I77" s="129"/>
-      <c r="J77" s="117"/>
-    </row>
-    <row r="78" spans="1:321" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F77" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="81"/>
+      <c r="H77" s="81"/>
+      <c r="I77" s="82"/>
+      <c r="J77" s="88"/>
+    </row>
+    <row r="78" spans="1:321" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="36"/>
-      <c r="C78" s="65"/>
-      <c r="D78" s="127"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="95"/>
       <c r="E78" s="34" t="s">
         <v>8</v>
       </c>
@@ -3075,27 +3075,27 @@
       <c r="I78" s="60">
         <v>0.7</v>
       </c>
-      <c r="J78" s="118"/>
-    </row>
-    <row r="79" spans="1:321" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J78" s="89"/>
+    </row>
+    <row r="79" spans="1:321" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="49"/>
       <c r="B79" s="48"/>
-      <c r="C79" s="64">
+      <c r="C79" s="70">
         <v>34</v>
       </c>
-      <c r="D79" s="142" t="s">
+      <c r="D79" s="79" t="s">
         <v>27</v>
       </c>
       <c r="E79" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G79" s="109"/>
-      <c r="H79" s="109"/>
-      <c r="I79" s="110"/>
-      <c r="J79" s="107"/>
+      <c r="F79" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="66"/>
+      <c r="H79" s="66"/>
+      <c r="I79" s="67"/>
+      <c r="J79" s="63"/>
       <c r="K79" s="49"/>
       <c r="L79" s="49"/>
       <c r="M79" s="49"/>
@@ -3408,11 +3408,11 @@
       <c r="LH79" s="49"/>
       <c r="LI79" s="49"/>
     </row>
-    <row r="80" spans="1:321" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:321" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="49"/>
       <c r="B80" s="48"/>
-      <c r="C80" s="65"/>
-      <c r="D80" s="123"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="75"/>
       <c r="E80" s="34" t="s">
         <v>8</v>
       </c>
@@ -3428,7 +3428,7 @@
       <c r="I80" s="58">
         <v>0.7</v>
       </c>
-      <c r="J80" s="108"/>
+      <c r="J80" s="64"/>
       <c r="K80" s="49"/>
       <c r="L80" s="49"/>
       <c r="M80" s="49"/>
@@ -3741,29 +3741,29 @@
       <c r="LH80" s="49"/>
       <c r="LI80" s="49"/>
     </row>
-    <row r="81" spans="2:10" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:10" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="53"/>
-      <c r="C81" s="64">
+      <c r="C81" s="70">
         <v>35</v>
       </c>
-      <c r="D81" s="145" t="s">
+      <c r="D81" s="72" t="s">
         <v>28</v>
       </c>
       <c r="E81" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F81" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G81" s="109"/>
-      <c r="H81" s="109"/>
-      <c r="I81" s="110"/>
-      <c r="J81" s="107"/>
-    </row>
-    <row r="82" spans="2:10" s="54" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F81" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="66"/>
+      <c r="H81" s="66"/>
+      <c r="I81" s="67"/>
+      <c r="J81" s="63"/>
+    </row>
+    <row r="82" spans="2:10" s="54" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B82" s="53"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="143"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="73"/>
       <c r="E82" s="34" t="s">
         <v>8</v>
       </c>
@@ -3779,31 +3779,31 @@
       <c r="I82" s="58">
         <v>0.7</v>
       </c>
-      <c r="J82" s="108"/>
-    </row>
-    <row r="83" spans="2:10" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J82" s="64"/>
+    </row>
+    <row r="83" spans="2:10" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="53"/>
-      <c r="C83" s="64">
+      <c r="C83" s="70">
         <v>36</v>
       </c>
-      <c r="D83" s="145" t="s">
+      <c r="D83" s="72" t="s">
         <v>68</v>
       </c>
       <c r="E83" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F83" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G83" s="109"/>
-      <c r="H83" s="109"/>
-      <c r="I83" s="110"/>
-      <c r="J83" s="107"/>
-    </row>
-    <row r="84" spans="2:10" s="54" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F83" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G83" s="66"/>
+      <c r="H83" s="66"/>
+      <c r="I83" s="67"/>
+      <c r="J83" s="63"/>
+    </row>
+    <row r="84" spans="2:10" s="54" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="53"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="143"/>
+      <c r="C84" s="71"/>
+      <c r="D84" s="73"/>
       <c r="E84" s="34" t="s">
         <v>8</v>
       </c>
@@ -3819,31 +3819,31 @@
       <c r="I84" s="58">
         <v>0.7</v>
       </c>
-      <c r="J84" s="108"/>
-    </row>
-    <row r="85" spans="2:10" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J84" s="64"/>
+    </row>
+    <row r="85" spans="2:10" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="26"/>
-      <c r="C85" s="64">
+      <c r="C85" s="70">
         <v>36</v>
       </c>
-      <c r="D85" s="145" t="s">
+      <c r="D85" s="72" t="s">
         <v>69</v>
       </c>
       <c r="E85" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85" s="109"/>
-      <c r="H85" s="109"/>
-      <c r="I85" s="110"/>
-      <c r="J85" s="107"/>
-    </row>
-    <row r="86" spans="2:10" s="27" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F85" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="66"/>
+      <c r="H85" s="66"/>
+      <c r="I85" s="67"/>
+      <c r="J85" s="63"/>
+    </row>
+    <row r="86" spans="2:10" s="27" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="26"/>
-      <c r="C86" s="65"/>
-      <c r="D86" s="143"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="73"/>
       <c r="E86" s="34" t="s">
         <v>8</v>
       </c>
@@ -3859,31 +3859,31 @@
       <c r="I86" s="30">
         <v>0.7</v>
       </c>
-      <c r="J86" s="108"/>
-    </row>
-    <row r="87" spans="2:10" s="27" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J86" s="64"/>
+    </row>
+    <row r="87" spans="2:10" s="27" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="26"/>
-      <c r="C87" s="64">
+      <c r="C87" s="70">
         <v>37</v>
       </c>
-      <c r="D87" s="142" t="s">
+      <c r="D87" s="79" t="s">
         <v>34</v>
       </c>
       <c r="E87" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F87" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G87" s="109"/>
-      <c r="H87" s="109"/>
-      <c r="I87" s="110"/>
-      <c r="J87" s="107"/>
-    </row>
-    <row r="88" spans="2:10" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F87" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G87" s="66"/>
+      <c r="H87" s="66"/>
+      <c r="I87" s="67"/>
+      <c r="J87" s="63"/>
+    </row>
+    <row r="88" spans="2:10" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B88" s="26"/>
-      <c r="C88" s="65"/>
-      <c r="D88" s="123"/>
+      <c r="C88" s="71"/>
+      <c r="D88" s="75"/>
       <c r="E88" s="34" t="s">
         <v>8</v>
       </c>
@@ -3899,31 +3899,31 @@
       <c r="I88" s="58">
         <v>0.7</v>
       </c>
-      <c r="J88" s="108"/>
-    </row>
-    <row r="89" spans="2:10" s="54" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J88" s="64"/>
+    </row>
+    <row r="89" spans="2:10" s="54" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" s="53"/>
-      <c r="C89" s="64">
+      <c r="C89" s="70">
         <v>38</v>
       </c>
-      <c r="D89" s="122" t="s">
+      <c r="D89" s="74" t="s">
         <v>29</v>
       </c>
       <c r="E89" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F89" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G89" s="109"/>
-      <c r="H89" s="109"/>
-      <c r="I89" s="110"/>
-      <c r="J89" s="107"/>
-    </row>
-    <row r="90" spans="2:10" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F89" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G89" s="66"/>
+      <c r="H89" s="66"/>
+      <c r="I89" s="67"/>
+      <c r="J89" s="63"/>
+    </row>
+    <row r="90" spans="2:10" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="53"/>
-      <c r="C90" s="65"/>
-      <c r="D90" s="123"/>
+      <c r="C90" s="71"/>
+      <c r="D90" s="75"/>
       <c r="E90" s="34" t="s">
         <v>8</v>
       </c>
@@ -3939,31 +3939,31 @@
       <c r="I90" s="58">
         <v>0.7</v>
       </c>
-      <c r="J90" s="108"/>
-    </row>
-    <row r="91" spans="2:10" s="54" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J90" s="64"/>
+    </row>
+    <row r="91" spans="2:10" s="54" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="53"/>
-      <c r="C91" s="64">
+      <c r="C91" s="70">
         <v>39</v>
       </c>
-      <c r="D91" s="122" t="s">
+      <c r="D91" s="74" t="s">
         <v>35</v>
       </c>
       <c r="E91" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F91" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G91" s="109"/>
-      <c r="H91" s="109"/>
-      <c r="I91" s="110"/>
-      <c r="J91" s="107"/>
-    </row>
-    <row r="92" spans="2:10" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F91" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G91" s="66"/>
+      <c r="H91" s="66"/>
+      <c r="I91" s="67"/>
+      <c r="J91" s="63"/>
+    </row>
+    <row r="92" spans="2:10" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="53"/>
-      <c r="C92" s="65"/>
-      <c r="D92" s="123"/>
+      <c r="C92" s="71"/>
+      <c r="D92" s="75"/>
       <c r="E92" s="34" t="s">
         <v>8</v>
       </c>
@@ -3979,31 +3979,31 @@
       <c r="I92" s="58">
         <v>0.7</v>
       </c>
-      <c r="J92" s="108"/>
-    </row>
-    <row r="93" spans="2:10" s="27" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J92" s="64"/>
+    </row>
+    <row r="93" spans="2:10" s="27" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B93" s="26"/>
-      <c r="C93" s="64">
+      <c r="C93" s="70">
         <v>39</v>
       </c>
-      <c r="D93" s="122" t="s">
+      <c r="D93" s="74" t="s">
         <v>70</v>
       </c>
       <c r="E93" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F93" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G93" s="109"/>
-      <c r="H93" s="109"/>
-      <c r="I93" s="110"/>
-      <c r="J93" s="107"/>
-    </row>
-    <row r="94" spans="2:10" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F93" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G93" s="66"/>
+      <c r="H93" s="66"/>
+      <c r="I93" s="67"/>
+      <c r="J93" s="63"/>
+    </row>
+    <row r="94" spans="2:10" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="26"/>
-      <c r="C94" s="65"/>
-      <c r="D94" s="123"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="75"/>
       <c r="E94" s="34" t="s">
         <v>8</v>
       </c>
@@ -4019,31 +4019,31 @@
       <c r="I94" s="58">
         <v>0.7</v>
       </c>
-      <c r="J94" s="108"/>
-    </row>
-    <row r="95" spans="2:10" s="54" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J94" s="64"/>
+    </row>
+    <row r="95" spans="2:10" s="54" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="53"/>
-      <c r="C95" s="64">
+      <c r="C95" s="70">
         <v>40</v>
       </c>
-      <c r="D95" s="132" t="s">
+      <c r="D95" s="76" t="s">
         <v>30</v>
       </c>
       <c r="E95" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F95" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G95" s="109"/>
-      <c r="H95" s="109"/>
-      <c r="I95" s="110"/>
-      <c r="J95" s="107"/>
-    </row>
-    <row r="96" spans="2:10" s="54" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F95" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G95" s="66"/>
+      <c r="H95" s="66"/>
+      <c r="I95" s="67"/>
+      <c r="J95" s="63"/>
+    </row>
+    <row r="96" spans="2:10" s="54" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="53"/>
-      <c r="C96" s="65"/>
-      <c r="D96" s="143"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="73"/>
       <c r="E96" s="34" t="s">
         <v>8</v>
       </c>
@@ -4059,31 +4059,31 @@
       <c r="I96" s="58">
         <v>0.7</v>
       </c>
-      <c r="J96" s="108"/>
-    </row>
-    <row r="97" spans="2:10" s="54" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J96" s="64"/>
+    </row>
+    <row r="97" spans="2:10" s="54" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="53"/>
-      <c r="C97" s="64">
+      <c r="C97" s="70">
         <v>41</v>
       </c>
-      <c r="D97" s="132" t="s">
+      <c r="D97" s="76" t="s">
         <v>36</v>
       </c>
       <c r="E97" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F97" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G97" s="109"/>
-      <c r="H97" s="109"/>
-      <c r="I97" s="110"/>
-      <c r="J97" s="107"/>
-    </row>
-    <row r="98" spans="2:10" s="54" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F97" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G97" s="66"/>
+      <c r="H97" s="66"/>
+      <c r="I97" s="67"/>
+      <c r="J97" s="63"/>
+    </row>
+    <row r="98" spans="2:10" s="54" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="53"/>
-      <c r="C98" s="65"/>
-      <c r="D98" s="143"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="73"/>
       <c r="E98" s="34" t="s">
         <v>8</v>
       </c>
@@ -4099,29 +4099,29 @@
       <c r="I98" s="58">
         <v>0.7</v>
       </c>
-      <c r="J98" s="108"/>
-    </row>
-    <row r="99" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C99" s="64">
+      <c r="J98" s="64"/>
+    </row>
+    <row r="99" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C99" s="70">
         <v>42</v>
       </c>
-      <c r="D99" s="132" t="s">
+      <c r="D99" s="76" t="s">
         <v>31</v>
       </c>
       <c r="E99" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F99" s="135" t="s">
-        <v>7</v>
-      </c>
-      <c r="G99" s="136"/>
-      <c r="H99" s="136"/>
-      <c r="I99" s="137"/>
-      <c r="J99" s="134"/>
-    </row>
-    <row r="100" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C100" s="65"/>
-      <c r="D100" s="133"/>
+      <c r="F99" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="G99" s="86"/>
+      <c r="H99" s="86"/>
+      <c r="I99" s="87"/>
+      <c r="J99" s="84"/>
+    </row>
+    <row r="100" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C100" s="71"/>
+      <c r="D100" s="83"/>
       <c r="E100" s="34" t="s">
         <v>8</v>
       </c>
@@ -4137,31 +4137,31 @@
       <c r="I100" s="58">
         <v>0.7</v>
       </c>
-      <c r="J100" s="65"/>
-    </row>
-    <row r="101" spans="2:10" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J100" s="71"/>
+    </row>
+    <row r="101" spans="2:10" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="32"/>
-      <c r="C101" s="64">
+      <c r="C101" s="70">
         <v>43</v>
       </c>
-      <c r="D101" s="138" t="s">
+      <c r="D101" s="92" t="s">
         <v>32</v>
       </c>
       <c r="E101" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F101" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="G101" s="112"/>
-      <c r="H101" s="112"/>
-      <c r="I101" s="113"/>
-      <c r="J101" s="117"/>
-    </row>
-    <row r="102" spans="2:10" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F101" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G101" s="90"/>
+      <c r="H101" s="90"/>
+      <c r="I101" s="91"/>
+      <c r="J101" s="88"/>
+    </row>
+    <row r="102" spans="2:10" s="31" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B102" s="32"/>
-      <c r="C102" s="65"/>
-      <c r="D102" s="139"/>
+      <c r="C102" s="71"/>
+      <c r="D102" s="93"/>
       <c r="E102" s="34" t="s">
         <v>8</v>
       </c>
@@ -4177,31 +4177,31 @@
       <c r="I102" s="60">
         <v>0.7</v>
       </c>
-      <c r="J102" s="118"/>
-    </row>
-    <row r="103" spans="2:10" s="27" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J102" s="89"/>
+    </row>
+    <row r="103" spans="2:10" s="27" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="26"/>
-      <c r="C103" s="64">
+      <c r="C103" s="70">
         <v>44</v>
       </c>
-      <c r="D103" s="132" t="s">
+      <c r="D103" s="76" t="s">
         <v>37</v>
       </c>
       <c r="E103" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F103" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G103" s="109"/>
-      <c r="H103" s="109"/>
-      <c r="I103" s="110"/>
-      <c r="J103" s="107"/>
-    </row>
-    <row r="104" spans="2:10" s="27" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F103" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G103" s="66"/>
+      <c r="H103" s="66"/>
+      <c r="I103" s="67"/>
+      <c r="J103" s="63"/>
+    </row>
+    <row r="104" spans="2:10" s="27" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="26"/>
-      <c r="C104" s="65"/>
-      <c r="D104" s="143"/>
+      <c r="C104" s="71"/>
+      <c r="D104" s="73"/>
       <c r="E104" s="34" t="s">
         <v>8</v>
       </c>
@@ -4217,31 +4217,31 @@
       <c r="I104" s="58">
         <v>0.7</v>
       </c>
-      <c r="J104" s="108"/>
-    </row>
-    <row r="105" spans="2:10" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J104" s="64"/>
+    </row>
+    <row r="105" spans="2:10" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="53"/>
-      <c r="C105" s="64">
+      <c r="C105" s="70">
         <v>45</v>
       </c>
-      <c r="D105" s="142" t="s">
+      <c r="D105" s="79" t="s">
         <v>71</v>
       </c>
       <c r="E105" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F105" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G105" s="109"/>
-      <c r="H105" s="109"/>
-      <c r="I105" s="110"/>
-      <c r="J105" s="107"/>
-    </row>
-    <row r="106" spans="2:10" s="54" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F105" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G105" s="66"/>
+      <c r="H105" s="66"/>
+      <c r="I105" s="67"/>
+      <c r="J105" s="63"/>
+    </row>
+    <row r="106" spans="2:10" s="54" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B106" s="53"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="123"/>
+      <c r="C106" s="71"/>
+      <c r="D106" s="75"/>
       <c r="E106" s="34" t="s">
         <v>8</v>
       </c>
@@ -4257,31 +4257,31 @@
       <c r="I106" s="58">
         <v>0.7</v>
       </c>
-      <c r="J106" s="108"/>
-    </row>
-    <row r="107" spans="2:10" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J106" s="64"/>
+    </row>
+    <row r="107" spans="2:10" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="53"/>
-      <c r="C107" s="64">
+      <c r="C107" s="70">
         <v>46</v>
       </c>
-      <c r="D107" s="142" t="s">
+      <c r="D107" s="79" t="s">
         <v>72</v>
       </c>
       <c r="E107" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F107" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G107" s="109"/>
-      <c r="H107" s="109"/>
-      <c r="I107" s="110"/>
-      <c r="J107" s="107"/>
-    </row>
-    <row r="108" spans="2:10" s="54" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F107" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" s="66"/>
+      <c r="H107" s="66"/>
+      <c r="I107" s="67"/>
+      <c r="J107" s="63"/>
+    </row>
+    <row r="108" spans="2:10" s="54" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B108" s="53"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="123"/>
+      <c r="C108" s="71"/>
+      <c r="D108" s="75"/>
       <c r="E108" s="34" t="s">
         <v>8</v>
       </c>
@@ -4297,31 +4297,31 @@
       <c r="I108" s="58">
         <v>0.7</v>
       </c>
-      <c r="J108" s="108"/>
-    </row>
-    <row r="109" spans="2:10" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J108" s="64"/>
+    </row>
+    <row r="109" spans="2:10" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="53"/>
-      <c r="C109" s="64">
+      <c r="C109" s="70">
         <v>47</v>
       </c>
-      <c r="D109" s="142" t="s">
+      <c r="D109" s="79" t="s">
         <v>39</v>
       </c>
       <c r="E109" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F109" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G109" s="109"/>
-      <c r="H109" s="109"/>
-      <c r="I109" s="110"/>
-      <c r="J109" s="107"/>
-    </row>
-    <row r="110" spans="2:10" s="54" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F109" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G109" s="66"/>
+      <c r="H109" s="66"/>
+      <c r="I109" s="67"/>
+      <c r="J109" s="63"/>
+    </row>
+    <row r="110" spans="2:10" s="54" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B110" s="53"/>
-      <c r="C110" s="65"/>
-      <c r="D110" s="123"/>
+      <c r="C110" s="71"/>
+      <c r="D110" s="75"/>
       <c r="E110" s="34" t="s">
         <v>8</v>
       </c>
@@ -4337,31 +4337,31 @@
       <c r="I110" s="58">
         <v>0.7</v>
       </c>
-      <c r="J110" s="108"/>
-    </row>
-    <row r="111" spans="2:10" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J110" s="64"/>
+    </row>
+    <row r="111" spans="2:10" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="26"/>
-      <c r="C111" s="64">
+      <c r="C111" s="70">
         <v>48</v>
       </c>
-      <c r="D111" s="142" t="s">
+      <c r="D111" s="79" t="s">
         <v>38</v>
       </c>
       <c r="E111" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G111" s="109"/>
-      <c r="H111" s="109"/>
-      <c r="I111" s="110"/>
-      <c r="J111" s="107"/>
-    </row>
-    <row r="112" spans="2:10" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F111" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G111" s="66"/>
+      <c r="H111" s="66"/>
+      <c r="I111" s="67"/>
+      <c r="J111" s="63"/>
+    </row>
+    <row r="112" spans="2:10" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B112" s="26"/>
-      <c r="C112" s="65"/>
-      <c r="D112" s="123"/>
+      <c r="C112" s="71"/>
+      <c r="D112" s="75"/>
       <c r="E112" s="34" t="s">
         <v>8</v>
       </c>
@@ -4377,31 +4377,31 @@
       <c r="I112" s="58">
         <v>0.7</v>
       </c>
-      <c r="J112" s="108"/>
-    </row>
-    <row r="113" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J112" s="64"/>
+    </row>
+    <row r="113" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="53"/>
-      <c r="C113" s="64">
+      <c r="C113" s="70">
         <v>49</v>
       </c>
-      <c r="D113" s="140" t="s">
+      <c r="D113" s="68" t="s">
         <v>40</v>
       </c>
       <c r="E113" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F113" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G113" s="109"/>
-      <c r="H113" s="109"/>
-      <c r="I113" s="110"/>
-      <c r="J113" s="107"/>
-    </row>
-    <row r="114" spans="2:10" s="54" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F113" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G113" s="66"/>
+      <c r="H113" s="66"/>
+      <c r="I113" s="67"/>
+      <c r="J113" s="63"/>
+    </row>
+    <row r="114" spans="2:10" s="54" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B114" s="53"/>
-      <c r="C114" s="65"/>
-      <c r="D114" s="141"/>
+      <c r="C114" s="71"/>
+      <c r="D114" s="69"/>
       <c r="E114" s="34" t="s">
         <v>8</v>
       </c>
@@ -4417,31 +4417,31 @@
       <c r="I114" s="58">
         <v>0.7</v>
       </c>
-      <c r="J114" s="108"/>
-    </row>
-    <row r="115" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J114" s="64"/>
+    </row>
+    <row r="115" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B115" s="53"/>
-      <c r="C115" s="64">
+      <c r="C115" s="70">
         <v>50</v>
       </c>
-      <c r="D115" s="140" t="s">
+      <c r="D115" s="68" t="s">
         <v>41</v>
       </c>
       <c r="E115" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F115" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G115" s="109"/>
-      <c r="H115" s="109"/>
-      <c r="I115" s="110"/>
-      <c r="J115" s="107"/>
-    </row>
-    <row r="116" spans="2:10" s="54" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F115" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G115" s="66"/>
+      <c r="H115" s="66"/>
+      <c r="I115" s="67"/>
+      <c r="J115" s="63"/>
+    </row>
+    <row r="116" spans="2:10" s="54" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B116" s="53"/>
-      <c r="C116" s="65"/>
-      <c r="D116" s="141"/>
+      <c r="C116" s="71"/>
+      <c r="D116" s="69"/>
       <c r="E116" s="34" t="s">
         <v>8</v>
       </c>
@@ -4457,31 +4457,31 @@
       <c r="I116" s="58">
         <v>0.7</v>
       </c>
-      <c r="J116" s="108"/>
-    </row>
-    <row r="117" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J116" s="64"/>
+    </row>
+    <row r="117" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B117" s="53"/>
-      <c r="C117" s="64">
+      <c r="C117" s="70">
         <v>51</v>
       </c>
-      <c r="D117" s="140" t="s">
+      <c r="D117" s="68" t="s">
         <v>42</v>
       </c>
       <c r="E117" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F117" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G117" s="109"/>
-      <c r="H117" s="109"/>
-      <c r="I117" s="110"/>
-      <c r="J117" s="107"/>
-    </row>
-    <row r="118" spans="2:10" s="54" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F117" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G117" s="66"/>
+      <c r="H117" s="66"/>
+      <c r="I117" s="67"/>
+      <c r="J117" s="63"/>
+    </row>
+    <row r="118" spans="2:10" s="54" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B118" s="53"/>
-      <c r="C118" s="65"/>
-      <c r="D118" s="141"/>
+      <c r="C118" s="71"/>
+      <c r="D118" s="69"/>
       <c r="E118" s="34" t="s">
         <v>8</v>
       </c>
@@ -4494,34 +4494,34 @@
       <c r="H118" s="30">
         <v>0.5</v>
       </c>
-      <c r="I118" s="30">
-        <v>0.7</v>
-      </c>
-      <c r="J118" s="108"/>
-    </row>
-    <row r="119" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I118" s="58">
+        <v>0.7</v>
+      </c>
+      <c r="J118" s="64"/>
+    </row>
+    <row r="119" spans="2:10" s="54" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B119" s="53"/>
-      <c r="C119" s="64">
+      <c r="C119" s="70">
         <v>52</v>
       </c>
-      <c r="D119" s="140" t="s">
+      <c r="D119" s="68" t="s">
         <v>61</v>
       </c>
       <c r="E119" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F119" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G119" s="109"/>
-      <c r="H119" s="109"/>
-      <c r="I119" s="110"/>
-      <c r="J119" s="107"/>
-    </row>
-    <row r="120" spans="2:10" s="54" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F119" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G119" s="66"/>
+      <c r="H119" s="66"/>
+      <c r="I119" s="67"/>
+      <c r="J119" s="63"/>
+    </row>
+    <row r="120" spans="2:10" s="54" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="53"/>
-      <c r="C120" s="65"/>
-      <c r="D120" s="141"/>
+      <c r="C120" s="71"/>
+      <c r="D120" s="69"/>
       <c r="E120" s="34" t="s">
         <v>8</v>
       </c>
@@ -4537,31 +4537,31 @@
       <c r="I120" s="30">
         <v>0.7</v>
       </c>
-      <c r="J120" s="108"/>
-    </row>
-    <row r="121" spans="2:10" s="27" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J120" s="64"/>
+    </row>
+    <row r="121" spans="2:10" s="27" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B121" s="26"/>
-      <c r="C121" s="64">
+      <c r="C121" s="70">
         <v>53</v>
       </c>
-      <c r="D121" s="140" t="s">
+      <c r="D121" s="68" t="s">
         <v>62</v>
       </c>
       <c r="E121" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F121" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G121" s="109"/>
-      <c r="H121" s="109"/>
-      <c r="I121" s="110"/>
-      <c r="J121" s="107"/>
-    </row>
-    <row r="122" spans="2:10" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="F121" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G121" s="66"/>
+      <c r="H121" s="66"/>
+      <c r="I121" s="67"/>
+      <c r="J121" s="63"/>
+    </row>
+    <row r="122" spans="2:10" s="27" customFormat="1" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B122" s="26"/>
-      <c r="C122" s="65"/>
-      <c r="D122" s="141"/>
+      <c r="C122" s="71"/>
+      <c r="D122" s="69"/>
       <c r="E122" s="34" t="s">
         <v>8</v>
       </c>
@@ -4577,10 +4577,208 @@
       <c r="I122" s="30">
         <v>0.7</v>
       </c>
-      <c r="J122" s="108"/>
+      <c r="J122" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="222">
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:J62"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="J71:J72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="J73:J74"/>
+    <mergeCell ref="J75:J76"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="J69:J70"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="J99:J100"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="J101:J102"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="J87:J88"/>
+    <mergeCell ref="J85:J86"/>
+    <mergeCell ref="J89:J90"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="F119:I119"/>
+    <mergeCell ref="J119:J120"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="F117:I117"/>
+    <mergeCell ref="J117:J118"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="F109:I109"/>
+    <mergeCell ref="J109:J110"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="J113:J114"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="J111:J112"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="F115:I115"/>
+    <mergeCell ref="J115:J116"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="J93:J94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="J95:J96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="J107:J108"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="J103:J104"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="J81:J82"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="J77:J78"/>
     <mergeCell ref="J121:J122"/>
     <mergeCell ref="F121:I121"/>
     <mergeCell ref="D121:D122"/>
@@ -4605,204 +4803,6 @@
     <mergeCell ref="D87:D88"/>
     <mergeCell ref="J63:J64"/>
     <mergeCell ref="J79:J80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="J81:J82"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="J93:J94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="J95:J96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="J107:J108"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="J103:J104"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="D119:D120"/>
-    <mergeCell ref="F119:I119"/>
-    <mergeCell ref="J119:J120"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="F117:I117"/>
-    <mergeCell ref="J117:J118"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="F109:I109"/>
-    <mergeCell ref="J109:J110"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="F113:I113"/>
-    <mergeCell ref="J113:J114"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="J111:J112"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="F115:I115"/>
-    <mergeCell ref="J115:J116"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="J99:J100"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="J101:J102"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="J87:J88"/>
-    <mergeCell ref="J85:J86"/>
-    <mergeCell ref="J89:J90"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="J77:J78"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="J71:J72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="J73:J74"/>
-    <mergeCell ref="J75:J76"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="J69:J70"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="J61:J62"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="J2">
     <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Controlla se hai cancellato tutte le voci che non servono e se hai dato tutte le risposte">

</xml_diff>